<commit_message>
Changed cleaning to support additional data
</commit_message>
<xml_diff>
--- a/intervention/art_&_design_auto.xlsx
+++ b/intervention/art_&_design_auto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,61 +452,441 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>V931414517045</t>
+          <t>W931252509017</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N931253409013</t>
+          <t>T931252911047</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R931100609011</t>
+          <t>T931252110004</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>T931252911047</t>
+          <t>N931253409013</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>T931252110004</t>
+          <t>V931414517045</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>W931252509017</t>
+          <t>R931100609011</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>R931321009045</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>R931412017031</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>L931412020028</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>L931321113001</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>D931383810007</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>V931252909047</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Z931100609006</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>H931101008036</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Y931412017035</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>C931253110015</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>V931240110042</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>H931321309010</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>R931100609009</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>X931252710015</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>N931240110007</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>T931100609002</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>M931321110016</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>G936239910030</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>L931101008038</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>M888201710014</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>D931252109051</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>V802229210007</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>D931100608056</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>C931316110004</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>A931259308039</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>G931259509014</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>J931101108070</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>K931100609063</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>G931321110032</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>W931321110033</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>V931412017033</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>V931321008075</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>U931325209009</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>W310350110023</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>W931254310067</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>F931100509027</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>D931325309031</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>B931400418001</t>
         </is>
       </c>
     </row>

</xml_diff>